<commit_message>
Fig 2 and updated correlations for degree added
</commit_message>
<xml_diff>
--- a/results/Tbl2.xlsx
+++ b/results/Tbl2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Tbl2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Means by Sample</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Methods-Degree</t>
   </si>
   <si>
-    <t>other degrees =0</t>
-  </si>
-  <si>
     <t>Stats-Skill</t>
   </si>
   <si>
@@ -158,6 +155,12 @@
   </si>
   <si>
     <t>Team Aspects</t>
+  </si>
+  <si>
+    <t>Sociology Degree</t>
+  </si>
+  <si>
+    <t>political science =0</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +332,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -693,7 +709,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -718,9 +734,6 @@
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
@@ -730,11 +743,20 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1058,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1088,16 +1110,16 @@
       <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1106,22 +1128,22 @@
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1146,7 +1168,7 @@
       <c r="E5" s="9">
         <v>0.92420140768814296</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>1</v>
       </c>
       <c r="G5" s="10"/>
@@ -1171,7 +1193,7 @@
       <c r="F6" s="9">
         <v>0.37019976605402899</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>1</v>
       </c>
       <c r="H6" s="10"/>
@@ -1181,7 +1203,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9">
         <v>1.37933114035088E-2</v>
@@ -1198,14 +1220,14 @@
       <c r="G7" s="9">
         <v>-0.35231294058902501</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="I7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
     </row>
     <row r="8" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
@@ -1218,13 +1240,13 @@
       <c r="F8" s="11"/>
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="15" t="s">
+      <c r="I8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1244,16 +1266,16 @@
       <c r="E9" s="9">
         <v>0.94214652608813199</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="14">
+      <c r="F9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="13">
         <v>1</v>
       </c>
       <c r="J9" s="10"/>
@@ -1275,19 +1297,19 @@
       <c r="E10" s="9">
         <v>0.68559070018923995</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>27</v>
+      <c r="F10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="I10" s="9">
         <v>0.36592346752576299</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <v>1</v>
       </c>
       <c r="K10" s="10"/>
@@ -1297,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="9">
         <v>1.0922149122807E-2</v>
@@ -1308,14 +1330,14 @@
       <c r="E11" s="9">
         <v>1.9180346039470102E-2</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>27</v>
+      <c r="F11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="I11" s="9">
         <v>-0.61676764599865697</v>
@@ -1323,7 +1345,7 @@
       <c r="J11" s="9">
         <v>-0.53058293569961201</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1350,171 +1372,171 @@
         <v>16</v>
       </c>
       <c r="C13" s="9">
-        <v>0.68421052631578905</v>
+        <v>0.66666666666666696</v>
       </c>
       <c r="D13" s="9">
         <v>0.62032085561497297</v>
       </c>
       <c r="E13" s="9">
-        <v>0.65186789388197097</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0.13209152938298399</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0.20376046424361499</v>
-      </c>
-      <c r="H13" s="9">
-        <v>-0.110005799007352</v>
-      </c>
-      <c r="I13" s="9">
-        <v>0.157076904511736</v>
-      </c>
-      <c r="J13" s="9">
-        <v>0.21112355433188801</v>
-      </c>
-      <c r="K13" s="9">
-        <v>-0.21107215467307699</v>
+        <v>0.64350614644575099</v>
+      </c>
+      <c r="F13" s="19">
+        <v>0.13239236712616201</v>
+      </c>
+      <c r="G13" s="19">
+        <v>0.21716027607709501</v>
+      </c>
+      <c r="H13" s="19">
+        <v>-0.10800163567839</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0.15926995778908601</v>
+      </c>
+      <c r="J13" s="19">
+        <v>0.224564813090668</v>
+      </c>
+      <c r="K13" s="19">
+        <v>-0.21364707140356701</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9">
-        <v>2.6315789473684199E-2</v>
+        <v>0.487179487179487</v>
       </c>
       <c r="D14" s="9">
-        <v>6.0109289617486301E-2</v>
+        <v>0.51122994652406395</v>
       </c>
       <c r="E14" s="9">
-        <v>4.3240284619594997E-2</v>
+        <v>0.49919828968466101</v>
       </c>
       <c r="F14" s="9">
-        <v>-0.136215276872383</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="G14" s="9">
-        <v>-9.4008137666967403E-2</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="H14" s="9">
-        <v>2.4216456076799699E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I14" s="9">
-        <v>-0.17380231379045399</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="J14" s="9">
-        <v>-0.126049440670085</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="K14" s="9">
-        <v>0.19685701113978299</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C15" s="9">
-        <v>4.9507263194944499E-3</v>
+        <v>-4.7117150475679298E-2</v>
       </c>
       <c r="D15" s="9">
-        <v>0.120284182595185</v>
+        <v>9.3341971986106304E-2</v>
       </c>
       <c r="E15" s="9">
-        <v>6.3335556648552505E-2</v>
+        <v>2.30748749127598E-2</v>
       </c>
       <c r="F15" s="9">
-        <v>-3.8551535239970902E-2</v>
+        <v>-2.1797393345218598E-3</v>
       </c>
       <c r="G15" s="9">
-        <v>-4.9776951062752803E-2</v>
-      </c>
-      <c r="H15" s="9">
-        <v>-2.0008699664839699E-2</v>
+        <v>-3.5880144803052801E-2</v>
+      </c>
+      <c r="H15" s="19">
+        <v>-4.85034623929987E-2</v>
       </c>
       <c r="I15" s="9">
-        <v>-9.7994945357630994E-3</v>
+        <v>1.2517203911143E-3</v>
       </c>
       <c r="J15" s="9">
-        <v>-3.0399070891402299E-2</v>
+        <v>-2.42553266975872E-2</v>
       </c>
       <c r="K15" s="9">
-        <v>7.4168243682424303E-3</v>
+        <v>2.4556098664601498E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C16" s="9">
-        <v>-6.9767441860465101E-2</v>
+        <v>-8.84615384615383E-2</v>
       </c>
       <c r="D16" s="9">
-        <v>-8.9168013928618093E-3</v>
+        <v>1.87165775401083E-3</v>
       </c>
       <c r="E16" s="9">
-        <v>-3.8963246496518701E-2</v>
-      </c>
-      <c r="F16" s="9">
-        <v>-0.21765748926519199</v>
-      </c>
-      <c r="G16" s="9">
-        <v>-0.208205742471677</v>
+        <v>-4.33190807055049E-2</v>
+      </c>
+      <c r="F16" s="19">
+        <v>-0.1758085470455</v>
+      </c>
+      <c r="G16" s="19">
+        <v>-0.22579963953034701</v>
       </c>
       <c r="H16" s="9">
-        <v>8.24154809624318E-2</v>
-      </c>
-      <c r="I16" s="9">
-        <v>-0.23062892643004501</v>
-      </c>
-      <c r="J16" s="9">
-        <v>-0.16909483858594701</v>
-      </c>
-      <c r="K16" s="9">
-        <v>0.25933368224598702</v>
+        <v>-8.3952245824994599E-3</v>
+      </c>
+      <c r="I16" s="19">
+        <v>-0.220878289351253</v>
+      </c>
+      <c r="J16" s="19">
+        <v>-0.23950917543810701</v>
+      </c>
+      <c r="K16" s="19">
+        <v>0.28856441472671701</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C17" s="9">
-        <v>2.07894736842105</v>
+        <v>2.1025641025641</v>
       </c>
       <c r="D17" s="9">
         <v>2.25294117647059</v>
       </c>
       <c r="E17" s="9">
-        <v>2.1670276123443402</v>
+        <v>2.1777124532335601</v>
       </c>
       <c r="F17" s="9">
-        <v>-3.4050776042606798E-2</v>
+        <v>-3.6019175485613897E-2</v>
       </c>
       <c r="G17" s="9">
-        <v>1.03317352595894E-2</v>
-      </c>
-      <c r="H17" s="9">
-        <v>6.8533202130564394E-2</v>
+        <v>-4.1771470727436201E-3</v>
+      </c>
+      <c r="H17" s="19">
+        <v>6.7445150282106001E-2</v>
       </c>
       <c r="I17" s="9">
-        <v>-2.98290624374986E-2</v>
+        <v>-3.4334271064533198E-2</v>
       </c>
       <c r="J17" s="9">
-        <v>2.6668144448807801E-2</v>
+        <v>1.1326340171023099E-2</v>
       </c>
       <c r="K17" s="9">
-        <v>2.4366099860448202E-3</v>
+        <v>7.1968161912747E-3</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1522,34 +1544,34 @@
         <v>3</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="13">
+        <v>24</v>
+      </c>
+      <c r="C18" s="12">
         <v>1</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="12">
         <v>0</v>
       </c>
-      <c r="E18" s="13">
-        <v>0.493773687060097</v>
-      </c>
-      <c r="F18" s="13">
-        <v>0.117132846558009</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.29971432725403901</v>
-      </c>
-      <c r="H18" s="13">
-        <v>-0.19184106941700199</v>
-      </c>
-      <c r="I18" s="13">
-        <v>7.9963790370989593E-2</v>
-      </c>
-      <c r="J18" s="13">
-        <v>0.26960322213481402</v>
-      </c>
-      <c r="K18" s="13">
-        <v>-0.17207294269780199</v>
+      <c r="E18" s="12">
+        <v>0.50026723677177998</v>
+      </c>
+      <c r="F18" s="20">
+        <v>0.112808163578066</v>
+      </c>
+      <c r="G18" s="20">
+        <v>0.28164194153608002</v>
+      </c>
+      <c r="H18" s="20">
+        <v>-0.191027673485404</v>
+      </c>
+      <c r="I18" s="20">
+        <v>7.3433185174883703E-2</v>
+      </c>
+      <c r="J18" s="20">
+        <v>0.25101851582384599</v>
+      </c>
+      <c r="K18" s="20">
+        <v>-0.16581806469236501</v>
       </c>
     </row>
   </sheetData>
@@ -1567,759 +1589,759 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="17"/>
+    <col min="1" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="E2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="I2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>10</v>
+      </c>
+      <c r="B10" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>12</v>
+      </c>
+      <c r="B12" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>13</v>
+      </c>
+      <c r="B13" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>16</v>
+      </c>
+      <c r="B14" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>17</v>
+      </c>
+      <c r="B15" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>18</v>
+      </c>
+      <c r="B16" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>19</v>
+      </c>
+      <c r="B17" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>20</v>
+      </c>
+      <c r="B18" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>21</v>
+      </c>
+      <c r="B19" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>22</v>
+      </c>
+      <c r="B20" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>23</v>
+      </c>
+      <c r="B21" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>26</v>
+      </c>
+      <c r="B22" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>27</v>
+      </c>
+      <c r="B23" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>28</v>
+      </c>
+      <c r="B24" s="15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>29</v>
+      </c>
+      <c r="B25" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>30</v>
+      </c>
+      <c r="B26" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>31</v>
+      </c>
+      <c r="B27" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>32</v>
+      </c>
+      <c r="B28" s="15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>33</v>
+      </c>
+      <c r="B29" s="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>34</v>
+      </c>
+      <c r="B30" s="15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>35</v>
+      </c>
+      <c r="B31" s="15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>36</v>
+      </c>
+      <c r="B32" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>37</v>
+      </c>
+      <c r="B33" s="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>38</v>
+      </c>
+      <c r="B34" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>39</v>
+      </c>
+      <c r="B35" s="15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>40</v>
+      </c>
+      <c r="B36" s="15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>41</v>
+      </c>
+      <c r="B37" s="15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>42</v>
+      </c>
+      <c r="B38" s="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>43</v>
+      </c>
+      <c r="B39" s="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>45</v>
+      </c>
+      <c r="B40" s="15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>46</v>
+      </c>
+      <c r="B41" s="15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>47</v>
+      </c>
+      <c r="B42" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>48</v>
+      </c>
+      <c r="B43" s="15">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>49</v>
+      </c>
+      <c r="B44" s="15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>50</v>
+      </c>
+      <c r="B45" s="15">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>52</v>
+      </c>
+      <c r="B46" s="15">
         <v>44</v>
       </c>
-      <c r="M1" s="17" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>53</v>
+      </c>
+      <c r="B47" s="15">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>2</v>
-      </c>
-      <c r="B4" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>5</v>
-      </c>
-      <c r="B6" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>6</v>
-      </c>
-      <c r="B7" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>7</v>
-      </c>
-      <c r="B8" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>8</v>
-      </c>
-      <c r="B9" s="17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>10</v>
-      </c>
-      <c r="B10" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <v>11</v>
-      </c>
-      <c r="B11" s="17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>12</v>
-      </c>
-      <c r="B12" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>13</v>
-      </c>
-      <c r="B13" s="17">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <v>16</v>
-      </c>
-      <c r="B14" s="17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <v>17</v>
-      </c>
-      <c r="B15" s="17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>18</v>
-      </c>
-      <c r="B16" s="17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
-        <v>19</v>
-      </c>
-      <c r="B17" s="17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <v>20</v>
-      </c>
-      <c r="B18" s="17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
-        <v>21</v>
-      </c>
-      <c r="B19" s="17">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
-        <v>22</v>
-      </c>
-      <c r="B20" s="17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
-        <v>23</v>
-      </c>
-      <c r="B21" s="17">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
-        <v>26</v>
-      </c>
-      <c r="B22" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
-        <v>27</v>
-      </c>
-      <c r="B23" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
-        <v>28</v>
-      </c>
-      <c r="B24" s="17">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
-        <v>29</v>
-      </c>
-      <c r="B25" s="17">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
-        <v>30</v>
-      </c>
-      <c r="B26" s="17">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <v>31</v>
-      </c>
-      <c r="B27" s="17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
-        <v>32</v>
-      </c>
-      <c r="B28" s="17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
-        <v>33</v>
-      </c>
-      <c r="B29" s="17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
-        <v>34</v>
-      </c>
-      <c r="B30" s="17">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
-        <v>35</v>
-      </c>
-      <c r="B31" s="17">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
-        <v>36</v>
-      </c>
-      <c r="B32" s="17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
-        <v>37</v>
-      </c>
-      <c r="B33" s="17">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
-        <v>38</v>
-      </c>
-      <c r="B34" s="17">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
-        <v>39</v>
-      </c>
-      <c r="B35" s="17">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <v>40</v>
-      </c>
-      <c r="B36" s="17">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
-        <v>41</v>
-      </c>
-      <c r="B37" s="17">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
-        <v>42</v>
-      </c>
-      <c r="B38" s="17">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
-        <v>43</v>
-      </c>
-      <c r="B39" s="17">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
-        <v>45</v>
-      </c>
-      <c r="B40" s="17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <v>54</v>
+      </c>
+      <c r="B48" s="15">
         <v>46</v>
       </c>
-      <c r="B41" s="17">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <v>56</v>
+      </c>
+      <c r="B49" s="15">
         <v>47</v>
       </c>
-      <c r="B42" s="17">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>57</v>
+      </c>
+      <c r="B50" s="15">
         <v>48</v>
       </c>
-      <c r="B43" s="17">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>58</v>
+      </c>
+      <c r="B51" s="15">
         <v>49</v>
       </c>
-      <c r="B44" s="17">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>59</v>
+      </c>
+      <c r="B52" s="15">
         <v>50</v>
       </c>
-      <c r="B45" s="17">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>60</v>
+      </c>
+      <c r="B53" s="15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
+        <v>61</v>
+      </c>
+      <c r="B54" s="15">
         <v>52</v>
       </c>
-      <c r="B46" s="17">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>62</v>
+      </c>
+      <c r="B55" s="15">
         <v>53</v>
       </c>
-      <c r="B47" s="17">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>64</v>
+      </c>
+      <c r="B56" s="15">
         <v>54</v>
       </c>
-      <c r="B48" s="17">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>65</v>
+      </c>
+      <c r="B57" s="15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>67</v>
+      </c>
+      <c r="B58" s="15">
         <v>56</v>
       </c>
-      <c r="B49" s="17">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>68</v>
+      </c>
+      <c r="B59" s="15">
         <v>57</v>
       </c>
-      <c r="B50" s="17">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>69</v>
+      </c>
+      <c r="B60" s="15">
         <v>58</v>
       </c>
-      <c r="B51" s="17">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>70</v>
+      </c>
+      <c r="B61" s="15">
         <v>59</v>
       </c>
-      <c r="B52" s="17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
+        <v>72</v>
+      </c>
+      <c r="B62" s="15">
         <v>60</v>
       </c>
-      <c r="B53" s="17">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
+        <v>73</v>
+      </c>
+      <c r="B63" s="15">
         <v>61</v>
       </c>
-      <c r="B54" s="17">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>74</v>
+      </c>
+      <c r="B64" s="15">
         <v>62</v>
       </c>
-      <c r="B55" s="17">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>75</v>
+      </c>
+      <c r="B65" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>76</v>
+      </c>
+      <c r="B66" s="15">
         <v>64</v>
       </c>
-      <c r="B56" s="17">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>77</v>
+      </c>
+      <c r="B67" s="15">
         <v>65</v>
       </c>
-      <c r="B57" s="17">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>80</v>
+      </c>
+      <c r="B68" s="15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
+        <v>82</v>
+      </c>
+      <c r="B69" s="15">
         <v>67</v>
       </c>
-      <c r="B58" s="17">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="15">
+        <v>83</v>
+      </c>
+      <c r="B70" s="15">
         <v>68</v>
       </c>
-      <c r="B59" s="17">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="15">
+        <v>84</v>
+      </c>
+      <c r="B71" s="15">
         <v>69</v>
       </c>
-      <c r="B60" s="17">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="15">
+        <v>86</v>
+      </c>
+      <c r="B72" s="15">
         <v>70</v>
       </c>
-      <c r="B61" s="17">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="15">
+        <v>87</v>
+      </c>
+      <c r="B73" s="15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="15">
+        <v>88</v>
+      </c>
+      <c r="B74" s="15">
         <v>72</v>
       </c>
-      <c r="B62" s="17">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
+        <v>90</v>
+      </c>
+      <c r="B75" s="15">
         <v>73</v>
       </c>
-      <c r="B63" s="17">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="15">
+        <v>93</v>
+      </c>
+      <c r="B76" s="15">
         <v>74</v>
       </c>
-      <c r="B64" s="17">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="15">
+        <v>94</v>
+      </c>
+      <c r="B77" s="15">
         <v>75</v>
       </c>
-      <c r="B65" s="17">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="15">
+        <v>95</v>
+      </c>
+      <c r="B78" s="15">
         <v>76</v>
       </c>
-      <c r="B66" s="17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="15">
+        <v>96</v>
+      </c>
+      <c r="B79" s="15">
         <v>77</v>
       </c>
-      <c r="B67" s="17">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="15">
+        <v>97</v>
+      </c>
+      <c r="B80" s="15">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="15">
+        <v>98</v>
+      </c>
+      <c r="B81" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="15">
+        <v>101</v>
+      </c>
+      <c r="B82" s="15">
         <v>80</v>
       </c>
-      <c r="B68" s="17">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="15">
+        <v>102</v>
+      </c>
+      <c r="B83" s="15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="15">
+        <v>104</v>
+      </c>
+      <c r="B84" s="15">
         <v>82</v>
       </c>
-      <c r="B69" s="17">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="15">
+        <v>105</v>
+      </c>
+      <c r="B85" s="15">
         <v>83</v>
       </c>
-      <c r="B70" s="17">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="15">
+        <v>106</v>
+      </c>
+      <c r="B86" s="15">
         <v>84</v>
       </c>
-      <c r="B71" s="17">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
-        <v>86</v>
-      </c>
-      <c r="B72" s="17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
-        <v>87</v>
-      </c>
-      <c r="B73" s="17">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
-        <v>88</v>
-      </c>
-      <c r="B74" s="17">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
-        <v>90</v>
-      </c>
-      <c r="B75" s="17">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
-        <v>93</v>
-      </c>
-      <c r="B76" s="17">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="17">
-        <v>94</v>
-      </c>
-      <c r="B77" s="17">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="17">
-        <v>95</v>
-      </c>
-      <c r="B78" s="17">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="17">
-        <v>96</v>
-      </c>
-      <c r="B79" s="17">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="17">
-        <v>97</v>
-      </c>
-      <c r="B80" s="17">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
-        <v>98</v>
-      </c>
-      <c r="B81" s="17">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="15">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="17">
-        <v>101</v>
-      </c>
-      <c r="B82" s="17">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="17">
-        <v>102</v>
-      </c>
-      <c r="B83" s="17">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="17">
-        <v>104</v>
-      </c>
-      <c r="B84" s="17">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="17">
-        <v>105</v>
-      </c>
-      <c r="B85" s="17">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="17">
-        <v>106</v>
-      </c>
-      <c r="B86" s="17">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="17">
-        <v>79</v>
-      </c>
-      <c r="B87" s="17">
+      <c r="B87" s="15">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved on to Fig 2
</commit_message>
<xml_diff>
--- a/results/Tbl2.xlsx
+++ b/results/Tbl2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Means by Sample</t>
   </si>
@@ -43,18 +43,9 @@
     <t>Verification</t>
   </si>
   <si>
-    <t>Exact Verif.</t>
-  </si>
-  <si>
-    <t>Deviance</t>
-  </si>
-  <si>
     <t>Raw Replication Results</t>
   </si>
   <si>
-    <t>same direction =1</t>
-  </si>
-  <si>
     <t>Exact Verification</t>
   </si>
   <si>
@@ -164,6 +155,21 @@
   </si>
   <si>
     <t>routine variability =1</t>
+  </si>
+  <si>
+    <t>Exact Replication</t>
+  </si>
+  <si>
+    <t>Replication Error</t>
+  </si>
+  <si>
+    <t>Exact Rep.</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">same sign or NS diff. zero =1 </t>
   </si>
 </sst>
 </file>
@@ -1084,13 +1090,13 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:K18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="1" customWidth="1"/>
     <col min="3" max="5" width="9.6640625" style="1" customWidth="1"/>
     <col min="6" max="8" width="9.77734375" style="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" style="1" customWidth="1"/>
@@ -1119,7 +1125,7 @@
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
       <c r="F2" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
@@ -1132,7 +1138,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>4</v>
@@ -1141,18 +1147,18 @@
         <v>5</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1160,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C5" s="9">
         <v>0.95559210526315796</v>
@@ -1179,10 +1185,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9">
         <v>0.77247807017543901</v>
@@ -1203,10 +1209,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="9">
         <v>1.37933114035088E-2</v>
@@ -1227,14 +1233,14 @@
         <v>1</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
     <row r="8" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="11"/>
@@ -1244,13 +1250,13 @@
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
       <c r="I8" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -1258,7 +1264,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C9" s="9">
         <v>0.961074561403509</v>
@@ -1270,13 +1276,13 @@
         <v>0.94214652608813199</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I9" s="13">
         <v>1</v>
@@ -1286,10 +1292,10 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="9">
         <v>0.8125</v>
@@ -1301,13 +1307,13 @@
         <v>0.68559070018923995</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I10" s="9">
         <v>0.36592346752576299</v>
@@ -1319,10 +1325,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" s="9">
         <v>1.0922149122807E-2</v>
@@ -1334,13 +1340,13 @@
         <v>1.9180346039470102E-2</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I11" s="9">
         <v>-0.61676764599865697</v>
@@ -1354,7 +1360,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="11"/>
@@ -1369,10 +1375,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" s="9">
         <v>0.66666666666666696</v>
@@ -1404,10 +1410,10 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="9">
         <v>0.487179487179487</v>
@@ -1439,10 +1445,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9">
         <v>-4.7117150475679298E-2</v>
@@ -1474,10 +1480,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="9">
         <v>-8.84615384615383E-2</v>
@@ -1509,10 +1515,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" s="9">
         <v>2.1025641025641</v>
@@ -1544,10 +1550,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="9">
         <v>0.30769230769230799</v>
@@ -1582,13 +1588,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E19" s="12">
         <v>0.50026723677177998</v>
@@ -1638,66 +1644,66 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>39</v>
-      </c>
       <c r="K1" s="15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="F2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="H2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>41</v>
-      </c>
       <c r="J2" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>20</v>
-      </c>
       <c r="P2" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="16" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
adding qualitative categories to main descriptive table
</commit_message>
<xml_diff>
--- a/results/Tbl2.xlsx
+++ b/results/Tbl2.xlsx
@@ -1089,23 +1089,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="9.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="5" width="9.6328125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="9.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.08984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1118,7 +1118,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C2" s="20" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1130,7 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1156,12 +1156,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1169,13 +1169,13 @@
         <v>49</v>
       </c>
       <c r="C5" s="9">
-        <v>0.95559210526315796</v>
+        <v>0.95673076923076905</v>
       </c>
       <c r="D5" s="9">
-        <v>0.89358288770053496</v>
+        <v>0.89274279615795105</v>
       </c>
       <c r="E5" s="9">
-        <v>0.92420140768814296</v>
+        <v>0.92471970101441503</v>
       </c>
       <c r="F5" s="13">
         <v>1</v>
@@ -1183,7 +1183,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
@@ -1191,23 +1191,23 @@
         <v>9</v>
       </c>
       <c r="C6" s="9">
-        <v>0.77247807017543901</v>
+        <v>0.76923076923076905</v>
       </c>
       <c r="D6" s="9">
-        <v>0.48235294117647098</v>
+        <v>0.48132337246531498</v>
       </c>
       <c r="E6" s="9">
-        <v>0.62560909583107704</v>
+        <v>0.62520021356113198</v>
       </c>
       <c r="F6" s="9">
-        <v>0.37019976605402899</v>
+        <v>0.368506798064694</v>
       </c>
       <c r="G6" s="13">
         <v>1</v>
       </c>
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
@@ -1215,19 +1215,19 @@
         <v>22</v>
       </c>
       <c r="C7" s="9">
-        <v>1.37933114035088E-2</v>
+        <v>1.3442841880341901E-2</v>
       </c>
       <c r="D7" s="9">
-        <v>7.0771711229946493E-2</v>
+        <v>7.1198025613660607E-2</v>
       </c>
       <c r="E7" s="9">
-        <v>4.2637276664861903E-2</v>
+        <v>4.2335851575013399E-2</v>
       </c>
       <c r="F7" s="9">
-        <v>-0.30147856614827301</v>
+        <v>-0.30339833920210701</v>
       </c>
       <c r="G7" s="9">
-        <v>-0.35231294058902501</v>
+        <v>-0.35145586599592599</v>
       </c>
       <c r="H7" s="13">
         <v>1</v>
@@ -1238,7 +1238,7 @@
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
     </row>
-    <row r="8" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1267,13 +1267,13 @@
         <v>49</v>
       </c>
       <c r="C9" s="9">
-        <v>0.961074561403509</v>
+        <v>0.98183760683760701</v>
       </c>
       <c r="D9" s="9">
-        <v>0.92373333333333296</v>
+        <v>0.92320000000000002</v>
       </c>
       <c r="E9" s="9">
-        <v>0.94214652608813199</v>
+        <v>0.952495329597011</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>23</v>
@@ -1290,7 +1290,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>45</v>
       </c>
@@ -1298,13 +1298,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="9">
-        <v>0.8125</v>
+        <v>0.83867521367521403</v>
       </c>
       <c r="D10" s="9">
-        <v>0.56213333333333304</v>
+        <v>0.56640000000000001</v>
       </c>
       <c r="E10" s="9">
-        <v>0.68559070018923995</v>
+        <v>0.70242860955430997</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>23</v>
@@ -1316,14 +1316,14 @@
         <v>23</v>
       </c>
       <c r="I10" s="9">
-        <v>0.36592346752576299</v>
+        <v>0.34311699992622902</v>
       </c>
       <c r="J10" s="13">
         <v>1</v>
       </c>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -1331,13 +1331,13 @@
         <v>22</v>
       </c>
       <c r="C11" s="9">
-        <v>1.0922149122807E-2</v>
+        <v>7.9059829059829109E-3</v>
       </c>
       <c r="D11" s="9">
-        <v>2.7213919999999999E-2</v>
+        <v>2.4960053333333301E-2</v>
       </c>
       <c r="E11" s="9">
-        <v>1.9180346039470102E-2</v>
+        <v>1.6439845209500901E-2</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>23</v>
@@ -1349,16 +1349,16 @@
         <v>23</v>
       </c>
       <c r="I11" s="9">
-        <v>-0.61676764599865697</v>
+        <v>-0.59412614636768402</v>
       </c>
       <c r="J11" s="9">
-        <v>-0.53058293569961201</v>
+        <v>-0.51623280717746001</v>
       </c>
       <c r="K11" s="13">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1384,31 +1384,31 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="D13" s="9">
-        <v>0.62032085561497297</v>
+        <v>0.62113127001067203</v>
       </c>
       <c r="E13" s="9">
-        <v>0.64350614644575099</v>
+        <v>0.64388681260010705</v>
       </c>
       <c r="F13" s="18">
-        <v>0.13239236712616201</v>
+        <v>0.12376790047937999</v>
       </c>
       <c r="G13" s="18">
-        <v>0.21716027607709501</v>
+        <v>0.19810516144152601</v>
       </c>
       <c r="H13" s="18">
-        <v>-0.10800163567839</v>
+        <v>-0.10231112016204599</v>
       </c>
       <c r="I13" s="18">
-        <v>0.13848163909518199</v>
+        <v>0.103837549767532</v>
       </c>
       <c r="J13" s="18">
-        <v>0.18460673126316901</v>
+        <v>0.160972424171552</v>
       </c>
       <c r="K13" s="18">
-        <v>-0.16996610200571</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-0.14422922540153299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1419,31 +1419,31 @@
         <v>0.487179487179487</v>
       </c>
       <c r="D14" s="9">
-        <v>0.51122994652406395</v>
+        <v>0.51013874066168596</v>
       </c>
       <c r="E14" s="9">
-        <v>0.49919828968466101</v>
+        <v>0.49866524292578801</v>
       </c>
       <c r="F14" s="9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="G14" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H14" s="9">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I14" s="9">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G14" s="9">
-        <v>-2.1000000000000001E-2</v>
-      </c>
-      <c r="H14" s="9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="I14" s="9">
-        <v>3.3000000000000002E-2</v>
-      </c>
       <c r="J14" s="9">
-        <v>-1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="K14" s="18">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1454,31 +1454,31 @@
         <v>-4.7117150475679298E-2</v>
       </c>
       <c r="D15" s="9">
-        <v>9.3341971986106304E-2</v>
+        <v>9.2115702438429897E-2</v>
       </c>
       <c r="E15" s="9">
-        <v>2.30748749127598E-2</v>
+        <v>2.25364443884533E-2</v>
       </c>
       <c r="F15" s="9">
-        <v>-2.1797393345218598E-3</v>
+        <v>-3.2905955757696701E-3</v>
       </c>
       <c r="G15" s="9">
-        <v>-3.5880144803052801E-2</v>
+        <v>-3.9227299744986503E-2</v>
       </c>
       <c r="H15" s="18">
-        <v>-4.85034623929987E-2</v>
+        <v>-4.8086160442769303E-2</v>
       </c>
       <c r="I15" s="9">
-        <v>6.0716562246929803E-3</v>
+        <v>1.6806875767996499E-2</v>
       </c>
       <c r="J15" s="9">
-        <v>-2.1746832699885501E-2</v>
+        <v>-1.6632681423158099E-2</v>
       </c>
       <c r="K15" s="9">
-        <v>2.8166082927555598E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-6.8409280398918698E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1489,31 +1489,31 @@
         <v>-8.84615384615383E-2</v>
       </c>
       <c r="D16" s="9">
-        <v>1.87165775401083E-3</v>
+        <v>7.0971184631805004E-3</v>
       </c>
       <c r="E16" s="9">
-        <v>-4.33190807055049E-2</v>
+        <v>-4.0656700480512398E-2</v>
       </c>
       <c r="F16" s="18">
-        <v>-0.1758085470455</v>
+        <v>-0.18596892237794899</v>
       </c>
       <c r="G16" s="18">
-        <v>-0.22579963953034701</v>
+        <v>-0.239321783172534</v>
       </c>
       <c r="H16" s="9">
-        <v>-8.3952245824994599E-3</v>
+        <v>-4.3541696298016901E-4</v>
       </c>
       <c r="I16" s="18">
-        <v>-0.223924717717223</v>
+        <v>-0.218509776636481</v>
       </c>
       <c r="J16" s="18">
-        <v>-0.238591629296936</v>
+        <v>-0.230293303138601</v>
       </c>
       <c r="K16" s="18">
-        <v>0.29226900591558103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.28927945091004498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
@@ -1524,31 +1524,31 @@
         <v>2.1025641025641</v>
       </c>
       <c r="D17" s="9">
-        <v>2.25294117647059</v>
+        <v>2.2502668089647799</v>
       </c>
       <c r="E17" s="9">
-        <v>2.1777124532335601</v>
+        <v>2.17645488521089</v>
       </c>
       <c r="F17" s="9">
-        <v>-3.6019175485613897E-2</v>
+        <v>-3.49595818002763E-2</v>
       </c>
       <c r="G17" s="9">
-        <v>-4.1771470727436201E-3</v>
+        <v>-5.2701263715252402E-3</v>
       </c>
       <c r="H17" s="18">
-        <v>6.7445150282106001E-2</v>
+        <v>6.5457370395907696E-2</v>
       </c>
       <c r="I17" s="9">
-        <v>-4.0295999576945303E-2</v>
+        <v>-9.2519768141899605E-3</v>
       </c>
       <c r="J17" s="9">
-        <v>4.0721795901872398E-3</v>
+        <v>2.2059540783782201E-2</v>
       </c>
       <c r="K17" s="9">
-        <v>1.79277124782838E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>-5.1540426483950002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -1556,34 +1556,34 @@
         <v>44</v>
       </c>
       <c r="C18" s="9">
-        <v>0.30769230769230799</v>
+        <v>0.35897435897435898</v>
       </c>
       <c r="D18" s="9">
-        <v>0.74652406417112305</v>
+        <v>0.70224119530416196</v>
       </c>
       <c r="E18" s="9">
-        <v>0.52699091394975905</v>
+        <v>0.53069941270688703</v>
       </c>
       <c r="F18" s="18">
-        <v>-8.1000000000000003E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G18" s="18">
-        <v>-0.34300000000000003</v>
+        <v>-0.23699999999999999</v>
       </c>
       <c r="H18" s="9">
-        <v>3.1E-2</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="I18" s="18">
-        <v>-7.3999999999999996E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="J18" s="18">
-        <v>-0.34499999999999997</v>
+        <v>-0.17899999999999999</v>
       </c>
       <c r="K18" s="18">
-        <v>0.22800000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>-2.7E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="6" t="s">
         <v>3</v>
       </c>
@@ -1597,25 +1597,25 @@
         <v>23</v>
       </c>
       <c r="E19" s="12">
-        <v>0.50026723677177998</v>
+        <v>0.49973304858515699</v>
       </c>
       <c r="F19" s="19">
-        <v>0.112808163578066</v>
+        <v>0.121261398612089</v>
       </c>
       <c r="G19" s="19">
-        <v>0.28164194153608002</v>
+        <v>0.29738122006328699</v>
       </c>
       <c r="H19" s="19">
-        <v>-0.191027673485404</v>
+        <v>-0.19551013660168101</v>
       </c>
       <c r="I19" s="19">
-        <v>9.86128466299349E-2</v>
+        <v>0.137830877260125</v>
       </c>
       <c r="J19" s="19">
-        <v>0.27684318999746599</v>
+        <v>0.29777023906931999</v>
       </c>
       <c r="K19" s="19">
-        <v>-0.170571445492912</v>
+        <v>-0.200825518271152</v>
       </c>
     </row>
   </sheetData>
@@ -1637,12 +1637,12 @@
       <selection activeCell="D89" sqref="D89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="16384" width="8.90625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D1" s="15" t="s">
         <v>30</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>10</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>11</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
         <v>12</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>13</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
         <v>16</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
         <v>17</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
         <v>18</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>19</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>20</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>21</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>22</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>23</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>26</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>27</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>28</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>29</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>30</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>31</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>32</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>33</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <v>34</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>35</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>36</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>37</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>38</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <v>39</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>40</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>41</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>42</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>43</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <v>45</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <v>46</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <v>47</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>48</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>49</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>50</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <v>52</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
         <v>53</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <v>54</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="15">
         <v>56</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="15">
         <v>57</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="15">
         <v>58</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <v>59</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="15">
         <v>60</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <v>61</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>62</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>64</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>65</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="15">
         <v>67</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="15">
         <v>68</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>69</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="15">
         <v>70</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>72</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>73</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>74</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>75</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>76</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <v>77</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>80</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <v>82</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <v>83</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <v>84</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="15">
         <v>86</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="15">
         <v>87</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>88</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="15">
         <v>90</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="15">
         <v>93</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="15">
         <v>94</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="15">
         <v>95</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>96</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="15">
         <v>97</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="15">
         <v>98</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="15">
         <v>101</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="15">
         <v>102</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="15">
         <v>104</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="15">
         <v>105</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="15">
         <v>106</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="15">
         <v>79</v>
       </c>

</xml_diff>